<commit_message>
Student Classes compilation results writes to excel file.
</commit_message>
<xml_diff>
--- a/COMP2603Marker/output-test/706003586/Assignment_2_Makring_Slip.xlsx
+++ b/COMP2603Marker/output-test/706003586/Assignment_2_Makring_Slip.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>STUDENT ID</t>
   </si>
@@ -27,6 +27,36 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Compilation</t>
+  </si>
+  <si>
+    <t>Device.java</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Complies</t>
+  </si>
+  <si>
+    <t>PortableDevice.java</t>
+  </si>
+  <si>
+    <t>AC.java</t>
+  </si>
+  <si>
+    <t>Fan.java</t>
+  </si>
+  <si>
+    <t>StandingFan.java</t>
+  </si>
+  <si>
+    <t>CeilingFan.java</t>
+  </si>
+  <si>
+    <t>Room.java</t>
+  </si>
+  <si>
+    <t>CoolingSimulation.java</t>
   </si>
   <si>
     <t>Test Class</t>
@@ -127,13 +157,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="15.38671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="23.4140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="26.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.51953125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="6.46875" customWidth="true" bestFit="true"/>
@@ -164,36 +194,105 @@
       <c r="A4" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="3">
-        <v>7</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B6" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="B7" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="3">
+      <c r="B8" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>13</v>
+      <c r="B15" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue2. Added manual marker for COMP2603 A2
</commit_message>
<xml_diff>
--- a/COMP2603Marker/output-test/706003586/Assignment_2_Makring_Slip.xlsx
+++ b/COMP2603Marker/output-test/706003586/Assignment_2_Makring_Slip.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>STUDENT ID</t>
   </si>
@@ -32,10 +32,13 @@
     <t>Compilation</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>Device.java</t>
   </si>
   <si>
-    <t xml:space="preserve"> Complies</t>
+    <t>Compiles</t>
   </si>
   <si>
     <t>PortableDevice.java</t>
@@ -59,15 +62,24 @@
     <t>CoolingSimulation.java</t>
   </si>
   <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>/5.0</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
     <t>Test Class</t>
   </si>
   <si>
     <t>Test Method</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>ACTest</t>
   </si>
   <si>
@@ -77,13 +89,52 @@
     <t>ID should increment by 1</t>
   </si>
   <si>
+    <t>73.0</t>
+  </si>
+  <si>
+    <t>/74.0</t>
+  </si>
+  <si>
+    <t>Additional Comments</t>
+  </si>
+  <si>
+    <t>Criteria</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Out of</t>
+  </si>
+  <si>
+    <t>Areas/Comments</t>
+  </si>
+  <si>
+    <t>Code Design</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>/16.0</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>/21.0</t>
+  </si>
+  <si>
     <t>Final Total</t>
   </si>
   <si>
-    <t>73.0</t>
-  </si>
-  <si>
-    <t>/74.0</t>
+    <t>99.0</t>
+  </si>
+  <si>
+    <t>/100.0</t>
   </si>
 </sst>
 </file>
@@ -157,7 +208,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -166,7 +217,8 @@
     <col min="1" max="1" width="23.4140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="26.16796875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.51953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="6.46875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.6875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="18.58984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -194,105 +246,200 @@
       <c r="A4" t="s" s="3">
         <v>5</v>
       </c>
+      <c r="B4" t="s" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s" s="3">
+      <c r="A13" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="C13" t="s" s="3">
+      <c r="C13" t="s" s="2">
         <v>17</v>
       </c>
+      <c r="D13" t="s" s="2">
+        <v>18</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s" s="2">
+      <c r="A14" t="s" s="3">
         <v>19</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="3">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s" s="3">
         <v>21</v>
       </c>
       <c r="C15" t="s" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="D15" t="s" s="3">
+      <c r="B16" t="s" s="2">
         <v>23</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s" s="3">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>